<commit_message>
[imp] 1. 升级依赖0.17.1 2. 更新groovy && excel 3. 修改 hzero-iam-menu 的租户管理员模板 名为组织管理员
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/init-data/hzero_admin/hzero_admin/hzero-service-route.xlsx
+++ b/src/main/resources/script/db/init-data/hzero_admin/hzero_admin/hzero-service-route.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="196">
   <si>
     <r>
       <rPr>
@@ -1995,7 +1995,7 @@
     <t>公式=外键引用</t>
   </si>
   <si>
-    <t>2020-05-29</t>
+    <t>2020-07-06</t>
   </si>
   <si>
     <t>hzero</t>
@@ -2205,12 +2205,6 @@
     <t>hadm_service-38</t>
   </si>
   <si>
-    <t>hzero-dpm</t>
-  </si>
-  <si>
-    <t>hadm_service-39</t>
-  </si>
-  <si>
     <t>hzero-open</t>
   </si>
   <si>
@@ -2431,12 +2425,6 @@
   </si>
   <si>
     <t>/hap/**</t>
-  </si>
-  <si>
-    <t>hdpm</t>
-  </si>
-  <si>
-    <t>/hdpm/**</t>
   </si>
   <si>
     <t>hopn</t>
@@ -3449,7 +3437,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M72"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3943,93 +3931,102 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39">
-      <c r="E39" t="s">
+    <row r="40">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" t="s">
         <v>121</v>
       </c>
-      <c r="F39" t="s">
+      <c r="D40" t="s" s="42">
         <v>122</v>
       </c>
-      <c r="G39" t="s">
-        <v>122</v>
-      </c>
-      <c r="H39" t="s">
-        <v>122</v>
+      <c r="E40" t="s" s="43">
+        <v>123</v>
+      </c>
+      <c r="F40" t="s" s="44">
+        <v>124</v>
+      </c>
+      <c r="G40" t="s">
+        <v>125</v>
+      </c>
+      <c r="H40" t="s" s="45">
+        <v>126</v>
+      </c>
+      <c r="I40" t="s" s="46">
+        <v>127</v>
+      </c>
+      <c r="J40" t="s">
+        <v>128</v>
+      </c>
+      <c r="K40" t="s">
+        <v>129</v>
+      </c>
+      <c r="L40" t="s">
+        <v>130</v>
+      </c>
+      <c r="M40" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" t="s">
-        <v>123</v>
-      </c>
-      <c r="D41" t="s" s="42">
-        <v>124</v>
-      </c>
-      <c r="E41" t="s" s="43">
-        <v>125</v>
-      </c>
-      <c r="F41" t="s" s="44">
-        <v>126</v>
+      <c r="E41" t="s">
+        <v>132</v>
+      </c>
+      <c r="F41">
+        <f>路由!$E$8</f>
       </c>
       <c r="G41" t="s">
-        <v>127</v>
-      </c>
-      <c r="H41" t="s" s="45">
-        <v>128</v>
-      </c>
-      <c r="I41" t="s" s="46">
-        <v>129</v>
-      </c>
-      <c r="J41" t="s">
-        <v>130</v>
+        <v>60</v>
+      </c>
+      <c r="H41" t="s">
+        <v>133</v>
+      </c>
+      <c r="I41" t="s">
+        <v>134</v>
       </c>
       <c r="K41" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="L41" t="s">
-        <v>132</v>
-      </c>
-      <c r="M41" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42">
       <c r="E42" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F42">
-        <f>路由!$E$8</f>
+        <f>路由!$E$9</f>
       </c>
       <c r="G42" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H42" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I42" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K42" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L42" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43">
       <c r="E43" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F43">
-        <f>路由!$E$9</f>
+        <f>路由!$E$10</f>
       </c>
       <c r="G43" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H43" t="s">
         <v>138</v>
@@ -4038,21 +4035,21 @@
         <v>139</v>
       </c>
       <c r="K43" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L43" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44">
       <c r="E44" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F44">
-        <f>路由!$E$10</f>
+        <f>路由!$E$11</f>
       </c>
       <c r="G44" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H44" t="s">
         <v>140</v>
@@ -4061,21 +4058,21 @@
         <v>141</v>
       </c>
       <c r="K44" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L44" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45">
       <c r="E45" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F45">
-        <f>路由!$E$11</f>
+        <f>路由!$E$12</f>
       </c>
       <c r="G45" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H45" t="s">
         <v>142</v>
@@ -4084,21 +4081,21 @@
         <v>143</v>
       </c>
       <c r="K45" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L45" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46">
       <c r="E46" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F46">
-        <f>路由!$E$12</f>
+        <f>路由!$E$13</f>
       </c>
       <c r="G46" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H46" t="s">
         <v>144</v>
@@ -4107,21 +4104,21 @@
         <v>145</v>
       </c>
       <c r="K46" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L46" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47">
       <c r="E47" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F47">
-        <f>路由!$E$13</f>
+        <f>路由!$E$14</f>
       </c>
       <c r="G47" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H47" t="s">
         <v>146</v>
@@ -4130,21 +4127,21 @@
         <v>147</v>
       </c>
       <c r="K47" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L47" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48">
       <c r="E48" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F48">
-        <f>路由!$E$14</f>
+        <f>路由!$E$15</f>
       </c>
       <c r="G48" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H48" t="s">
         <v>148</v>
@@ -4153,47 +4150,47 @@
         <v>149</v>
       </c>
       <c r="K48" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="L48" t="s">
-        <v>137</v>
+        <v>135</v>
+      </c>
+      <c r="M48" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="49">
       <c r="E49" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F49">
-        <f>路由!$E$15</f>
+        <f>路由!$E$16</f>
       </c>
       <c r="G49" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H49" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="I49" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="K49" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="L49" t="s">
-        <v>137</v>
-      </c>
-      <c r="M49" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50">
       <c r="E50" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F50">
-        <f>路由!$E$16</f>
+        <f>路由!$E$17</f>
       </c>
       <c r="G50" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H50" t="s">
         <v>154</v>
@@ -4202,21 +4199,21 @@
         <v>155</v>
       </c>
       <c r="K50" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L50" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51">
       <c r="E51" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F51">
-        <f>路由!$E$17</f>
+        <f>路由!$E$18</f>
       </c>
       <c r="G51" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H51" t="s">
         <v>156</v>
@@ -4225,21 +4222,21 @@
         <v>157</v>
       </c>
       <c r="K51" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L51" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52">
       <c r="E52" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F52">
-        <f>路由!$E$18</f>
+        <f>路由!$E$19</f>
       </c>
       <c r="G52" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H52" t="s">
         <v>158</v>
@@ -4248,21 +4245,21 @@
         <v>159</v>
       </c>
       <c r="K52" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L52" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53">
       <c r="E53" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F53">
-        <f>路由!$E$19</f>
+        <f>路由!$E$20</f>
       </c>
       <c r="G53" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H53" t="s">
         <v>160</v>
@@ -4271,21 +4268,21 @@
         <v>161</v>
       </c>
       <c r="K53" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L53" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54">
       <c r="E54" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F54">
-        <f>路由!$E$20</f>
+        <f>路由!$E$21</f>
       </c>
       <c r="G54" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H54" t="s">
         <v>162</v>
@@ -4294,21 +4291,21 @@
         <v>163</v>
       </c>
       <c r="K54" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L54" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55">
       <c r="E55" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F55">
-        <f>路由!$E$21</f>
+        <f>路由!$E$22</f>
       </c>
       <c r="G55" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H55" t="s">
         <v>164</v>
@@ -4317,21 +4314,21 @@
         <v>165</v>
       </c>
       <c r="K55" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L55" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56">
       <c r="E56" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F56">
-        <f>路由!$E$22</f>
+        <f>路由!$E$23</f>
       </c>
       <c r="G56" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H56" t="s">
         <v>166</v>
@@ -4340,21 +4337,21 @@
         <v>167</v>
       </c>
       <c r="K56" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L56" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="57">
       <c r="E57" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F57">
-        <f>路由!$E$23</f>
+        <f>路由!$E$24</f>
       </c>
       <c r="G57" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H57" t="s">
         <v>168</v>
@@ -4363,21 +4360,21 @@
         <v>169</v>
       </c>
       <c r="K57" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L57" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="58">
       <c r="E58" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F58">
-        <f>路由!$E$24</f>
+        <f>路由!$E$25</f>
       </c>
       <c r="G58" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H58" t="s">
         <v>170</v>
@@ -4386,21 +4383,21 @@
         <v>171</v>
       </c>
       <c r="K58" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="L58" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59">
       <c r="E59" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F59">
-        <f>路由!$E$25</f>
+        <f>路由!$E$27</f>
       </c>
       <c r="G59" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="H59" t="s">
         <v>172</v>
@@ -4409,21 +4406,21 @@
         <v>173</v>
       </c>
       <c r="K59" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="L59" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="60">
       <c r="E60" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F60">
-        <f>路由!$E$27</f>
+        <f>路由!$E$28</f>
       </c>
       <c r="G60" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H60" t="s">
         <v>174</v>
@@ -4432,21 +4429,21 @@
         <v>175</v>
       </c>
       <c r="K60" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L60" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61">
       <c r="E61" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F61">
-        <f>路由!$E$28</f>
+        <f>路由!$E$29</f>
       </c>
       <c r="G61" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H61" t="s">
         <v>176</v>
@@ -4455,21 +4452,21 @@
         <v>177</v>
       </c>
       <c r="K61" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L61" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62">
       <c r="E62" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F62">
-        <f>路由!$E$29</f>
+        <f>路由!$E$30</f>
       </c>
       <c r="G62" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H62" t="s">
         <v>178</v>
@@ -4478,21 +4475,21 @@
         <v>179</v>
       </c>
       <c r="K62" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="L62" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="63">
       <c r="E63" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F63">
-        <f>路由!$E$30</f>
+        <f>路由!$E$31</f>
       </c>
       <c r="G63" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H63" t="s">
         <v>180</v>
@@ -4501,21 +4498,21 @@
         <v>181</v>
       </c>
       <c r="K63" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="L63" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64">
       <c r="E64" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F64">
-        <f>路由!$E$31</f>
+        <f>路由!$E$32</f>
       </c>
       <c r="G64" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H64" t="s">
         <v>182</v>
@@ -4524,21 +4521,21 @@
         <v>183</v>
       </c>
       <c r="K64" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L64" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65">
       <c r="E65" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F65">
-        <f>路由!$E$32</f>
+        <f>路由!$E$33</f>
       </c>
       <c r="G65" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H65" t="s">
         <v>184</v>
@@ -4547,21 +4544,21 @@
         <v>185</v>
       </c>
       <c r="K65" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L65" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66">
       <c r="E66" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F66">
-        <f>路由!$E$33</f>
+        <f>路由!$E$34</f>
       </c>
       <c r="G66" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H66" t="s">
         <v>186</v>
@@ -4570,21 +4567,21 @@
         <v>187</v>
       </c>
       <c r="K66" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L66" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67">
       <c r="E67" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F67">
-        <f>路由!$E$34</f>
+        <f>路由!$E$35</f>
       </c>
       <c r="G67" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H67" t="s">
         <v>188</v>
@@ -4593,21 +4590,21 @@
         <v>189</v>
       </c>
       <c r="K67" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L67" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68">
       <c r="E68" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F68">
-        <f>路由!$E$35</f>
+        <f>路由!$E$36</f>
       </c>
       <c r="G68" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H68" t="s">
         <v>190</v>
@@ -4616,21 +4613,21 @@
         <v>191</v>
       </c>
       <c r="K68" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L68" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69">
       <c r="E69" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F69">
-        <f>路由!$E$36</f>
+        <f>路由!$E$37</f>
       </c>
       <c r="G69" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H69" t="s">
         <v>192</v>
@@ -4639,21 +4636,21 @@
         <v>193</v>
       </c>
       <c r="K69" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="L69" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70">
       <c r="E70" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F70">
-        <f>路由!$E$37</f>
+        <f>路由!$E$38</f>
       </c>
       <c r="G70" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H70" t="s">
         <v>194</v>
@@ -4662,56 +4659,10 @@
         <v>195</v>
       </c>
       <c r="K70" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="L70" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="E71" t="s">
-        <v>134</v>
-      </c>
-      <c r="F71">
-        <f>路由!$E$38</f>
-      </c>
-      <c r="G71" t="s">
-        <v>120</v>
-      </c>
-      <c r="H71" t="s">
-        <v>196</v>
-      </c>
-      <c r="I71" t="s">
-        <v>197</v>
-      </c>
-      <c r="K71" t="s">
-        <v>137</v>
-      </c>
-      <c r="L71" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="E72" t="s">
-        <v>134</v>
-      </c>
-      <c r="F72">
-        <f>路由!$E$39</f>
-      </c>
-      <c r="G72" t="s">
-        <v>122</v>
-      </c>
-      <c r="H72" t="s">
-        <v>198</v>
-      </c>
-      <c r="I72" t="s">
-        <v>199</v>
-      </c>
-      <c r="K72" t="s">
-        <v>137</v>
-      </c>
-      <c r="L72" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>